<commit_message>
Integrating phpexcel. Understanding and testing the import system.
</commit_message>
<xml_diff>
--- a/files/test.xlsx
+++ b/files/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="9030" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -496,9 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -680,7 +678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>